<commit_message>
updating and adding abrade
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>Baz Widget</t>
+  </si>
+  <si>
+    <t>Biz Widget</t>
   </si>
 </sst>
 </file>
@@ -125,6 +128,14 @@
         <v>300.0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>400.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>